<commit_message>
created ClueGame that shows the whole game layout and an emoty GameBoardPanel class
</commit_message>
<xml_diff>
--- a/ClueLayout.xlsx
+++ b/ClueLayout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avely\eclipse\ClueGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9BED0B6-8736-4D34-BCA2-D4A872072D06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{914549A1-199D-46A8-891E-9B4899C2FB65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-24120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{451E3A58-194B-4F49-BAFE-E45E5B9C6614}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1557" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1550" uniqueCount="38">
   <si>
     <t>B</t>
   </si>
@@ -150,28 +150,7 @@
     <t>L#</t>
   </si>
   <si>
-    <t>Number of doors: 20</t>
-  </si>
-  <si>
-    <t>Light Grey: door direction tests (in BoardInitTests)</t>
-  </si>
-  <si>
-    <t>Magenta: room test</t>
-  </si>
-  <si>
-    <t>Light Green: adjacency secret passage</t>
-  </si>
-  <si>
     <t>W&lt;</t>
-  </si>
-  <si>
-    <t>Dark Green: Test adjacency (only walkways/empty)</t>
-  </si>
-  <si>
-    <t>Gold - Test targets</t>
-  </si>
-  <si>
-    <t>Orange - Test Occupied</t>
   </si>
 </sst>
 </file>
@@ -195,7 +174,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -246,12 +225,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -264,25 +237,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFD72DB3"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="6" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -299,7 +254,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -312,10 +267,8 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3229,8 +3182,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F767267-3641-42CE-9A8E-2B42BE0695CE}">
   <dimension ref="A1:AJ29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="AG17" sqref="AG17"/>
+    <sheetView tabSelected="1" topLeftCell="U1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="AG1" sqref="AG1:AI8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3333,11 +3286,9 @@
       <c r="AF1" s="1">
         <v>30</v>
       </c>
-      <c r="AG1" s="1"/>
-      <c r="AH1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AI1" s="1"/>
+      <c r="AG1" s="12"/>
+      <c r="AH1" s="13"/>
+      <c r="AI1" s="12"/>
       <c r="AJ1" s="1"/>
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.25">
@@ -3371,7 +3322,7 @@
       <c r="J2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="K2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L2" s="2" t="s">
@@ -3434,12 +3385,12 @@
       <c r="AE2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="AF2" s="10" t="s">
+      <c r="AF2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="AH2" s="11" t="s">
-        <v>38</v>
-      </c>
+      <c r="AG2" s="13"/>
+      <c r="AH2" s="13"/>
+      <c r="AI2" s="13"/>
     </row>
     <row r="3" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
@@ -3538,9 +3489,9 @@
       <c r="AF3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="AH3" s="12" t="s">
-        <v>39</v>
-      </c>
+      <c r="AG3" s="13"/>
+      <c r="AH3" s="13"/>
+      <c r="AI3" s="13"/>
     </row>
     <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
@@ -3639,9 +3590,9 @@
       <c r="AF4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="AH4" s="10" t="s">
-        <v>40</v>
-      </c>
+      <c r="AG4" s="13"/>
+      <c r="AH4" s="13"/>
+      <c r="AI4" s="13"/>
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
@@ -3716,8 +3667,8 @@
       <c r="X5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="Y5" s="11" t="s">
-        <v>41</v>
+      <c r="Y5" s="10" t="s">
+        <v>37</v>
       </c>
       <c r="Z5" s="2" t="s">
         <v>6</v>
@@ -3734,15 +3685,15 @@
       <c r="AD5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="AE5" s="12" t="s">
+      <c r="AE5" s="6" t="s">
         <v>11</v>
       </c>
       <c r="AF5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="AH5" s="9" t="s">
-        <v>42</v>
-      </c>
+      <c r="AG5" s="13"/>
+      <c r="AH5" s="13"/>
+      <c r="AI5" s="13"/>
     </row>
     <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
@@ -3766,7 +3717,7 @@
       <c r="G6" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="H6" s="9" t="s">
+      <c r="H6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="I6" s="4" t="s">
@@ -3787,7 +3738,7 @@
       <c r="N6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="O6" s="9" t="s">
+      <c r="O6" s="10" t="s">
         <v>12</v>
       </c>
       <c r="P6" s="4" t="s">
@@ -3841,9 +3792,9 @@
       <c r="AF6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="AH6" s="13" t="s">
-        <v>43</v>
-      </c>
+      <c r="AG6" s="13"/>
+      <c r="AH6" s="13"/>
+      <c r="AI6" s="13"/>
     </row>
     <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
@@ -3930,7 +3881,7 @@
       <c r="AB7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="AC7" s="11" t="s">
+      <c r="AC7" s="10" t="s">
         <v>13</v>
       </c>
       <c r="AD7" s="4" t="s">
@@ -3942,9 +3893,9 @@
       <c r="AF7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="AH7" s="14" t="s">
-        <v>44</v>
-      </c>
+      <c r="AG7" s="13"/>
+      <c r="AH7" s="13"/>
+      <c r="AI7" s="13"/>
     </row>
     <row r="8" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
@@ -3971,10 +3922,10 @@
       <c r="H8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I8" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="J8" s="11" t="s">
+      <c r="I8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J8" s="10" t="s">
         <v>12</v>
       </c>
       <c r="K8" s="2" t="s">
@@ -4004,7 +3955,7 @@
       <c r="S8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="T8" s="15" t="s">
+      <c r="T8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="U8" s="2" t="s">
@@ -4043,6 +3994,9 @@
       <c r="AF8" s="4" t="s">
         <v>3</v>
       </c>
+      <c r="AG8" s="13"/>
+      <c r="AH8" s="13"/>
+      <c r="AI8" s="13"/>
     </row>
     <row r="9" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
@@ -4081,7 +4035,7 @@
       <c r="L9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="M9" s="11" t="s">
+      <c r="M9" s="10" t="s">
         <v>13</v>
       </c>
       <c r="N9" s="4" t="s">
@@ -4114,8 +4068,8 @@
       <c r="W9" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="X9" s="15" t="s">
-        <v>41</v>
+      <c r="X9" s="11" t="s">
+        <v>37</v>
       </c>
       <c r="Y9" s="2" t="s">
         <v>6</v>
@@ -4123,7 +4077,7 @@
       <c r="Z9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="AA9" s="15" t="s">
+      <c r="AA9" s="2" t="s">
         <v>6</v>
       </c>
       <c r="AB9" s="2" t="s">
@@ -4262,7 +4216,7 @@
       <c r="G11" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H11" s="11" t="s">
+      <c r="H11" s="10" t="s">
         <v>18</v>
       </c>
       <c r="I11" s="2" t="s">
@@ -4322,7 +4276,7 @@
       <c r="AA11" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="AB11" s="11" t="s">
+      <c r="AB11" s="10" t="s">
         <v>18</v>
       </c>
       <c r="AC11" s="2" t="s">
@@ -4334,7 +4288,7 @@
       <c r="AE11" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="AF11" s="9" t="s">
+      <c r="AF11" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -4467,7 +4421,7 @@
       <c r="J13" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="K13" s="9" t="s">
+      <c r="K13" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L13" s="2" t="s">
@@ -4595,7 +4549,7 @@
       <c r="T14" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="U14" s="15" t="s">
+      <c r="U14" s="4" t="s">
         <v>15</v>
       </c>
       <c r="V14" s="4" t="s">
@@ -4607,7 +4561,7 @@
       <c r="X14" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="Y14" s="9" t="s">
+      <c r="Y14" s="2" t="s">
         <v>6</v>
       </c>
       <c r="Z14" s="4" t="s">
@@ -4636,7 +4590,7 @@
       <c r="A15" s="1">
         <v>13</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C15" s="2" t="s">
@@ -4648,7 +4602,7 @@
       <c r="E15" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F15" s="14" t="s">
+      <c r="F15" s="2" t="s">
         <v>6</v>
       </c>
       <c r="G15" s="2" t="s">
@@ -4743,19 +4697,19 @@
       <c r="D16" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E16" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="F16" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="G16" s="14" t="s">
+      <c r="E16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G16" s="2" t="s">
         <v>6</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I16" s="11" t="s">
+      <c r="I16" s="10" t="s">
         <v>18</v>
       </c>
       <c r="J16" s="2" t="s">
@@ -4832,7 +4786,7 @@
       <c r="A17" s="1">
         <v>15</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="10" t="s">
         <v>18</v>
       </c>
       <c r="C17" s="2" t="s">
@@ -4868,7 +4822,7 @@
       <c r="M17" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N17" s="11" t="s">
+      <c r="N17" s="10" t="s">
         <v>12</v>
       </c>
       <c r="O17" s="2" t="s">
@@ -4895,7 +4849,7 @@
       <c r="V17" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="W17" s="15" t="s">
+      <c r="W17" s="11" t="s">
         <v>12</v>
       </c>
       <c r="X17" s="2" t="s">
@@ -4975,10 +4929,10 @@
       <c r="P18" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="Q18" s="11" t="s">
+      <c r="Q18" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="R18" s="9" t="s">
+      <c r="R18" s="11" t="s">
         <v>18</v>
       </c>
       <c r="S18" s="2" t="s">
@@ -5230,13 +5184,13 @@
       <c r="C21" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D21" s="15" t="s">
+      <c r="D21" s="4" t="s">
         <v>26</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F21" s="11" t="s">
+      <c r="F21" s="10" t="s">
         <v>13</v>
       </c>
       <c r="G21" s="4" t="s">
@@ -5355,7 +5309,7 @@
       <c r="L22" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="M22" s="11" t="s">
+      <c r="M22" s="10" t="s">
         <v>13</v>
       </c>
       <c r="N22" s="4" t="s">
@@ -5382,8 +5336,8 @@
       <c r="U22" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="V22" s="11" t="s">
-        <v>41</v>
+      <c r="V22" s="10" t="s">
+        <v>37</v>
       </c>
       <c r="W22" s="2" t="s">
         <v>6</v>
@@ -5453,7 +5407,7 @@
       <c r="L23" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="M23" s="11" t="s">
+      <c r="M23" s="10" t="s">
         <v>13</v>
       </c>
       <c r="N23" s="4" t="s">
@@ -5480,8 +5434,8 @@
       <c r="U23" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="V23" s="11" t="s">
-        <v>41</v>
+      <c r="V23" s="10" t="s">
+        <v>37</v>
       </c>
       <c r="W23" s="2" t="s">
         <v>6</v>
@@ -5498,7 +5452,7 @@
       <c r="AA23" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="AB23" s="11" t="s">
+      <c r="AB23" s="10" t="s">
         <v>13</v>
       </c>
       <c r="AC23" s="4" t="s">
@@ -5518,7 +5472,7 @@
       <c r="A24" s="1">
         <v>22</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="B24" s="9" t="s">
         <v>34</v>
       </c>
       <c r="C24" s="4" t="s">
@@ -5551,7 +5505,7 @@
       <c r="L24" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="M24" s="15" t="s">
+      <c r="M24" s="2" t="s">
         <v>6</v>
       </c>
       <c r="N24" s="4" t="s">
@@ -5587,10 +5541,10 @@
       <c r="X24" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="Y24" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="Z24" s="14" t="s">
+      <c r="Y24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z24" s="2" t="s">
         <v>6</v>
       </c>
       <c r="AA24" s="2" t="s">
@@ -5723,7 +5677,7 @@
       <c r="D26" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E26" s="9" t="s">
+      <c r="E26" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F26" s="2" t="s">

</xml_diff>